<commit_message>
Updated rubric and various lecture notes
</commit_message>
<xml_diff>
--- a/LabStarters/Lab05/Lab5Rubric_8wk.xlsx
+++ b/LabStarters/Lab05/Lab5Rubric_8wk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3693362C-B9DE-1742-9E42-A3E4A6B92622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F618AE2F-2E27-2446-8E49-ADC7F9134D00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15760" yWindow="500" windowWidth="13040" windowHeight="13760" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="9900" yWindow="500" windowWidth="13040" windowHeight="16500" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Part 1: CSS Layout for the home page</t>
   </si>
   <si>
-    <t>Figures</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Padding, visible border, and margin</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>Uploaded to citstudent</t>
+  </si>
+  <si>
+    <t>Figures on each page</t>
   </si>
 </sst>
 </file>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,14 +600,14 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>3</v>
@@ -625,14 +625,14 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>4</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5</v>
@@ -705,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,12 +720,12 @@
     <col min="5" max="5" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -746,13 +746,15 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -762,8 +764,9 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -773,8 +776,9 @@
       <c r="C6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -784,8 +788,9 @@
       <c r="C7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -795,8 +800,9 @@
       <c r="C8" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -806,8 +812,9 @@
       <c r="C9" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -817,8 +824,9 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -830,13 +838,18 @@
         <f>SUM(C3:C10)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,8 +859,9 @@
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -857,17 +871,19 @@
       <c r="C15" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>3</v>
@@ -875,8 +891,9 @@
       <c r="C17" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -886,17 +903,19 @@
       <c r="C18" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>4</v>
@@ -904,10 +923,11 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -915,8 +935,9 @@
       <c r="C21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -926,10 +947,11 @@
       <c r="C22" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
         <v>5</v>
@@ -937,8 +959,9 @@
       <c r="C23" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -950,13 +973,15 @@
         <f>SUM(C15:C23)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -969,22 +994,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>

</xml_diff>